<commit_message>
create another train config yml with adapted patch stride shapes
</commit_message>
<xml_diff>
--- a/train3dunet-annotations.xlsx
+++ b/train3dunet-annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048E70CC-3286-4235-8135-5E097E19B2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62446DD5-FF40-4402-859A-2A326E19E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0F2D7A5E-81A0-4E3E-85AE-E3E4B5F8BF98}"/>
+    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{0F2D7A5E-81A0-4E3E-85AE-E3E4B5F8BF98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>date of training</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>input data format is valid; patch and stride shape settings produce patches without labels; conda virtual environment fixed (CUDA and pytorch installations fixed, versioning problem)</t>
+  </si>
+  <si>
+    <t>train_config-230829-0.yml</t>
+  </si>
+  <si>
+    <t>better performance metrics;</t>
+  </si>
+  <si>
+    <t>cluster.s3it.uzh.ch:~/data/outputs/chpt-230829-0/</t>
   </si>
 </sst>
 </file>
@@ -496,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE866AC3-C5E2-4954-81B9-B1A93CD6658C}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,6 +692,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q3">
     <sortCondition ref="A2:A3"/>

</xml_diff>

<commit_message>
complete annotations for aborted 230829-0 run
</commit_message>
<xml_diff>
--- a/train3dunet-annotations.xlsx
+++ b/train3dunet-annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62446DD5-FF40-4402-859A-2A326E19E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631ADE54-027A-4214-94A8-CABA11AF2167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{0F2D7A5E-81A0-4E3E-85AE-E3E4B5F8BF98}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>date of training</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>cluster.s3it.uzh.ch:~/data/outputs/chpt-230829-0/</t>
+  </si>
+  <si>
+    <t>resource not allocated:</t>
+  </si>
+  <si>
+    <t>resources not allocated (pending for hours)</t>
   </si>
 </sst>
 </file>
@@ -699,11 +705,44 @@
       <c r="B4" t="s">
         <v>30</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" t="s">
+        <v>16</v>
       </c>
       <c r="P4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
delete failed runs (including non git outputs on cluster via globus)
</commit_message>
<xml_diff>
--- a/train3dunet-annotations.xlsx
+++ b/train3dunet-annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631ADE54-027A-4214-94A8-CABA11AF2167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A73C6E-C986-445B-BB6A-AA467857DAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{0F2D7A5E-81A0-4E3E-85AE-E3E4B5F8BF98}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>date of training</t>
   </si>
@@ -56,9 +56,6 @@
     <t>output directory (checkpoint, console output, nvidia-smi)</t>
   </si>
   <si>
-    <t>models were produced</t>
-  </si>
-  <si>
     <t>incl. nvidia-smi output</t>
   </si>
   <si>
@@ -128,19 +125,10 @@
     <t>input data format is valid; patch and stride shape settings produce patches without labels; conda virtual environment fixed (CUDA and pytorch installations fixed, versioning problem)</t>
   </si>
   <si>
-    <t>train_config-230829-0.yml</t>
-  </si>
-  <si>
     <t>better performance metrics;</t>
   </si>
   <si>
-    <t>cluster.s3it.uzh.ch:~/data/outputs/chpt-230829-0/</t>
-  </si>
-  <si>
-    <t>resource not allocated:</t>
-  </si>
-  <si>
-    <t>resources not allocated (pending for hours)</t>
+    <t>models were produced (and saved/not deleted)</t>
   </si>
 </sst>
 </file>
@@ -511,28 +499,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE866AC3-C5E2-4954-81B9-B1A93CD6658C}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="166.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
     <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="84.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="77.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="53" bestFit="1" customWidth="1"/>
@@ -550,10 +538,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -562,31 +550,31 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>5</v>
@@ -597,7 +585,7 @@
         <v>45159</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -606,13 +594,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -627,22 +615,22 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -650,7 +638,7 @@
         <v>45166</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -659,13 +647,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -680,76 +668,35 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>45167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>32</v>
-      </c>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q3">

</xml_diff>